<commit_message>
DOCS - burndown update
</commit_message>
<xml_diff>
--- a/DOCS/Documentação das Sprints/burn3.xlsx
+++ b/DOCS/Documentação das Sprints/burn3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API-2\DOCS\Documentação das Sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A805C55E-8127-4477-AF48-8F3AA57F74A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07A0D59-B03F-4AA3-A6C3-CCAC144BFD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -928,58 +928,58 @@
                   <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1571,58 +1571,58 @@
                   <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2431,7 +2431,7 @@
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3121,7 +3121,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -3159,75 +3159,75 @@
       </c>
       <c r="E25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I25" s="4">
         <f>H25-SUM(I2:I24)</f>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L25" s="4">
         <f>K25-SUM(L2:L24)</f>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V25" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
DOCS - burndown 3
</commit_message>
<xml_diff>
--- a/DOCS/Documentação das Sprints/burn3.xlsx
+++ b/DOCS/Documentação das Sprints/burn3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API-2\DOCS\Documentação das Sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07A0D59-B03F-4AA3-A6C3-CCAC144BFD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C1D651-38E0-46F1-A96D-4FDE09F92479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Total de horas</t>
   </si>
@@ -108,55 +108,67 @@
     <t>Tasks</t>
   </si>
   <si>
-    <t>S0-Mudar status do usuário na edição do usuário</t>
-  </si>
-  <si>
-    <t>S1-Caso usuário esteja desativado, impedir login</t>
-  </si>
-  <si>
-    <t>S2-Tratamento de erros no login</t>
-  </si>
-  <si>
-    <t>S2.1-Realizar testes e aplicar tratamento correto de erros em todos os cadastros</t>
-  </si>
-  <si>
-    <t>S3-Pesquisar quais informações são relevantes para mostrar no dashboard</t>
-  </si>
-  <si>
-    <t>S4-Explorar possíveis mudanças no front-end</t>
-  </si>
-  <si>
-    <t>S5-Arrumar estimativas de cada User Story no README</t>
-  </si>
-  <si>
-    <t>S6-Atualizar tabela das sprints com link para cada documento de cada sprint no README</t>
-  </si>
-  <si>
     <t>S7-Colocar logos para cada tecnologia usada no README</t>
   </si>
   <si>
-    <t>S8-Gravar vídeo da sprint 2 e botar no README</t>
-  </si>
-  <si>
-    <t>S9-Dashboard para RH</t>
-  </si>
-  <si>
-    <t>S10-Dashboard para Gestor geral</t>
-  </si>
-  <si>
     <t>S11-Dashboard para Gestor de área</t>
   </si>
   <si>
     <t>S12-Dashboard para Colaborador</t>
   </si>
   <si>
-    <t>S13.2-Manual de instalação</t>
-  </si>
-  <si>
     <t>S13.1-Manual de usuário</t>
   </si>
   <si>
     <t>Gestão de git e docs (SM)</t>
+  </si>
+  <si>
+    <t>S14-Exportar dados de usuários para uma planilha excel</t>
+  </si>
+  <si>
+    <t>S15-Exportar dados de objetivos para uma planilha excel</t>
+  </si>
+  <si>
+    <t>S16-Exportar dados de PDIs para uma planilha excel</t>
+  </si>
+  <si>
+    <t>S17-Tela da equipe do gestor de área</t>
+  </si>
+  <si>
+    <t>S0-Mudar status do usuário na edição do usuário (concluida)</t>
+  </si>
+  <si>
+    <t>S1-Caso usuário esteja desativado, impedir login (concluida)</t>
+  </si>
+  <si>
+    <t>S2-Tratamento de erros no login (concluida)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S2.1-Realizar testes e aplicar tratamento correto de erros em todos os cadastros </t>
+  </si>
+  <si>
+    <t>S3-Pesquisar quais informações são relevantes para mostrar no dashboard (concluida)</t>
+  </si>
+  <si>
+    <t>S4-Melhorar a estilização do front</t>
+  </si>
+  <si>
+    <t>S5-Arrumar estimativas de cada User Story no README (concluida)</t>
+  </si>
+  <si>
+    <t>S6-Atualizar tabela das sprints com link para cada documento de cada sprint no README (concluida)</t>
+  </si>
+  <si>
+    <t>S8-Gravar vídeo da sprint 2 e botar no README (concluida)</t>
+  </si>
+  <si>
+    <t>S9-Dashboard para RH (concluida)</t>
+  </si>
+  <si>
+    <t>S10-Dashboard para Gestor geral (concluida)</t>
+  </si>
+  <si>
+    <t>S13.2-Manual de instalação (concluida)</t>
   </si>
 </sst>
 </file>
@@ -919,67 +931,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1093,64 +1105,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.1</c:v>
+                  <c:v>62.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.2</c:v>
+                  <c:v>59.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.3</c:v>
+                  <c:v>56.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46.4</c:v>
+                  <c:v>52.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43.5</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.6</c:v>
+                  <c:v>46.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37.700000000000003</c:v>
+                  <c:v>42.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34.799999999999997</c:v>
+                  <c:v>39.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.900000000000002</c:v>
+                  <c:v>36.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26.1</c:v>
+                  <c:v>29.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23.200000000000003</c:v>
+                  <c:v>26.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20.300000000000004</c:v>
+                  <c:v>23.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17.399999999999999</c:v>
+                  <c:v>19.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14.5</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.600000000000001</c:v>
+                  <c:v>13.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.7000000000000028</c:v>
+                  <c:v>9.9000000000000057</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.8000000000000043</c:v>
+                  <c:v>6.6000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.8999999999999986</c:v>
+                  <c:v>3.3000000000000043</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1562,67 +1574,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>50</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1736,64 +1748,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.1</c:v>
+                  <c:v>62.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.2</c:v>
+                  <c:v>59.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.3</c:v>
+                  <c:v>56.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46.4</c:v>
+                  <c:v>52.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43.5</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.6</c:v>
+                  <c:v>46.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37.700000000000003</c:v>
+                  <c:v>42.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34.799999999999997</c:v>
+                  <c:v>39.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.900000000000002</c:v>
+                  <c:v>36.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26.1</c:v>
+                  <c:v>29.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23.200000000000003</c:v>
+                  <c:v>26.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20.300000000000004</c:v>
+                  <c:v>23.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17.399999999999999</c:v>
+                  <c:v>19.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14.5</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.600000000000001</c:v>
+                  <c:v>13.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.7000000000000028</c:v>
+                  <c:v>9.9000000000000057</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.8000000000000043</c:v>
+                  <c:v>6.6000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.8999999999999986</c:v>
+                  <c:v>3.3000000000000043</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -2430,8 +2442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,7 +2525,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -2543,7 +2555,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -2573,7 +2585,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -2603,7 +2615,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
@@ -2615,7 +2627,9 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -2631,13 +2645,17 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -2659,7 +2677,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
@@ -2687,7 +2705,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -2702,7 +2720,9 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -2715,7 +2735,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -2728,7 +2748,9 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -2743,7 +2765,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -2772,13 +2794,15 @@
       <c r="V10" s="1"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
+      <c r="A11" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -2800,8 +2824,8 @@
       <c r="V11" s="1"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>34</v>
+      <c r="A12" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B12" s="1">
         <v>5</v>
@@ -2810,11 +2834,15 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1">
+        <v>3</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="K12" s="1">
+        <v>2</v>
+      </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -2829,7 +2857,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1">
         <v>5</v>
@@ -2838,11 +2866,15 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1">
+        <v>3</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="K13" s="1">
+        <v>2</v>
+      </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -2857,7 +2889,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1">
         <v>5</v>
@@ -2868,9 +2900,13 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
       <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -2885,7 +2921,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1">
         <v>5</v>
@@ -2896,9 +2932,13 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
       <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -2913,7 +2953,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1">
         <v>5</v>
@@ -2924,7 +2964,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="I16" s="2"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -2941,10 +2981,10 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2953,7 +2993,9 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="J17" s="1">
+        <v>2</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -2968,8 +3010,12 @@
       <c r="V17" s="1"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2992,8 +3038,12 @@
       <c r="V18" s="1"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -3003,7 +3053,9 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="L19" s="1">
+        <v>1.5</v>
+      </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -3016,8 +3068,12 @@
       <c r="V19" s="1"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -3040,8 +3096,12 @@
       <c r="V20" s="1"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1">
+        <v>5</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -3113,7 +3173,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1">
         <v>8</v>
@@ -3147,87 +3207,87 @@
       </c>
       <c r="B25" s="4">
         <f>SUM(B2:B24)</f>
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" ref="C25:V25" si="0">B25-SUM(C2:C24)</f>
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I25" s="4">
         <f>H25-SUM(I2:I24)</f>
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="L25" s="4">
         <f>K25-SUM(L2:L24)</f>
-        <v>50</v>
+        <v>34.5</v>
       </c>
       <c r="M25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>33.5</v>
       </c>
       <c r="N25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>33.5</v>
       </c>
       <c r="O25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>33.5</v>
       </c>
       <c r="P25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>33.5</v>
       </c>
       <c r="Q25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>33.5</v>
       </c>
       <c r="R25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>33.5</v>
       </c>
       <c r="S25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>33.5</v>
       </c>
       <c r="T25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>33.5</v>
       </c>
       <c r="U25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>33.5</v>
       </c>
       <c r="V25" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>33.5</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -3236,83 +3296,83 @@
       </c>
       <c r="B26" s="6">
         <f>SUM(B2:B24)</f>
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C26" s="6">
         <f>$B$26-(($B$26/20)*(COLUMN()-2))</f>
-        <v>55.1</v>
+        <v>62.7</v>
       </c>
       <c r="D26" s="6">
         <f t="shared" ref="D26:V26" si="1">$B$26-(($B$26/20)*(COLUMN()-2))</f>
-        <v>52.2</v>
+        <v>59.4</v>
       </c>
       <c r="E26" s="6">
         <f t="shared" si="1"/>
-        <v>49.3</v>
+        <v>56.1</v>
       </c>
       <c r="F26" s="6">
         <f t="shared" si="1"/>
-        <v>46.4</v>
+        <v>52.8</v>
       </c>
       <c r="G26" s="6">
         <f t="shared" si="1"/>
-        <v>43.5</v>
+        <v>49.5</v>
       </c>
       <c r="H26" s="6">
         <f t="shared" si="1"/>
-        <v>40.6</v>
+        <v>46.2</v>
       </c>
       <c r="I26" s="6">
         <f t="shared" si="1"/>
-        <v>37.700000000000003</v>
+        <v>42.900000000000006</v>
       </c>
       <c r="J26" s="6">
         <f t="shared" si="1"/>
-        <v>34.799999999999997</v>
+        <v>39.6</v>
       </c>
       <c r="K26" s="6">
         <f t="shared" si="1"/>
-        <v>31.900000000000002</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M26" s="6">
         <f t="shared" si="1"/>
-        <v>26.1</v>
+        <v>29.700000000000003</v>
       </c>
       <c r="N26" s="6">
         <f t="shared" si="1"/>
-        <v>23.200000000000003</v>
+        <v>26.400000000000006</v>
       </c>
       <c r="O26" s="6">
         <f t="shared" si="1"/>
-        <v>20.300000000000004</v>
+        <v>23.1</v>
       </c>
       <c r="P26" s="6">
         <f t="shared" si="1"/>
-        <v>17.399999999999999</v>
+        <v>19.800000000000004</v>
       </c>
       <c r="Q26" s="6">
         <f t="shared" si="1"/>
-        <v>14.5</v>
+        <v>16.5</v>
       </c>
       <c r="R26" s="6">
         <f t="shared" si="1"/>
-        <v>11.600000000000001</v>
+        <v>13.200000000000003</v>
       </c>
       <c r="S26" s="6">
         <f t="shared" si="1"/>
-        <v>8.7000000000000028</v>
+        <v>9.9000000000000057</v>
       </c>
       <c r="T26" s="6">
         <f t="shared" si="1"/>
-        <v>5.8000000000000043</v>
+        <v>6.6000000000000014</v>
       </c>
       <c r="U26" s="6">
         <f t="shared" si="1"/>
-        <v>2.8999999999999986</v>
+        <v>3.3000000000000043</v>
       </c>
       <c r="V26" s="6">
         <f t="shared" si="1"/>

</xml_diff>